<commit_message>
Added iso error validation.
</commit_message>
<xml_diff>
--- a/AccoutingProblem/App_Data/records/Livro1.xlsx
+++ b/AccoutingProblem/App_Data/records/Livro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C953DEAE-FDDA-45E1-B79E-E6799F8B6479}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CE3DDD-2D4A-4890-9C5D-71CF4ADA8099}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{A8472CF1-BA81-43A6-BEEF-29CC949645AE}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Account</t>
   </si>
@@ -51,6 +51,24 @@
   </si>
   <si>
     <t>EUR</t>
+  </si>
+  <si>
+    <t>Testing 2</t>
+  </si>
+  <si>
+    <t>asdfdsf</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Some description</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -403,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97DF8E5-5124-45A2-AC64-C21C3ABF6911}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -444,6 +462,34 @@
         <v>100</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>